<commit_message>
new branch ruslan added
</commit_message>
<xml_diff>
--- a/target/test-classes/Countries.xlsx
+++ b/target/test-classes/Countries.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>Country</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>Nur-Sultan</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -523,7 +529,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEE3AD6B-2764-CA44-8845-C5296D7C5983}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="394" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
@@ -542,6 +548,9 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -550,6 +559,9 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -558,6 +570,9 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -566,6 +581,9 @@
       <c r="B4" t="s">
         <v>47</v>
       </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -574,6 +592,9 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -582,6 +603,9 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -590,6 +614,9 @@
       <c r="B7" t="s">
         <v>42</v>
       </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -598,6 +625,9 @@
       <c r="B8" t="s">
         <v>13</v>
       </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -606,6 +636,9 @@
       <c r="B9" t="s">
         <v>15</v>
       </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -614,6 +647,9 @@
       <c r="B10" t="s">
         <v>17</v>
       </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -622,6 +658,9 @@
       <c r="B11" t="s">
         <v>27</v>
       </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -630,6 +669,9 @@
       <c r="B12" t="s">
         <v>20</v>
       </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -638,6 +680,9 @@
       <c r="B13" t="s">
         <v>22</v>
       </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -646,6 +691,9 @@
       <c r="B14" t="s">
         <v>23</v>
       </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -654,6 +702,9 @@
       <c r="B15" t="s">
         <v>26</v>
       </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -662,6 +713,9 @@
       <c r="B16" t="s">
         <v>41</v>
       </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -670,6 +724,9 @@
       <c r="B17" t="s">
         <v>44</v>
       </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -677,6 +734,9 @@
       </c>
       <c r="B18" t="s">
         <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>